<commit_message>
Update summary dynamic (windows,granularity) post adj.xlsx
</commit_message>
<xml_diff>
--- a/ForegroundJobScheduler/results/Nonoverlapping windows/summary dynamic (windows,granularity) post adj.xlsx
+++ b/ForegroundJobScheduler/results/Nonoverlapping windows/summary dynamic (windows,granularity) post adj.xlsx
@@ -10195,11 +10195,21 @@
       <c r="G306" t="n">
         <v>0.0</v>
       </c>
-      <c r="H306"/>
-      <c r="I306"/>
-      <c r="J306"/>
-      <c r="K306"/>
-      <c r="L306"/>
+      <c r="H306" t="n">
+        <v>0.1451146483726683</v>
+      </c>
+      <c r="I306" t="n">
+        <v>0.1424831084863354</v>
+      </c>
+      <c r="J306" t="n">
+        <v>0.9734308845016485</v>
+      </c>
+      <c r="K306" t="n">
+        <v>0.7901234567901234</v>
+      </c>
+      <c r="L306" t="n">
+        <v>0.6756315425763354</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="s">

</xml_diff>